<commit_message>
gitignored data folders and others
</commit_message>
<xml_diff>
--- a/Assignment_2/Workplan.xlsx
+++ b/Assignment_2/Workplan.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Data_Mining\DM_Techniques\Assignment_2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="14436" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Schedule for report</t>
   </si>
@@ -40,12 +45,18 @@
   </si>
   <si>
     <t>Recommender systems reading</t>
+  </si>
+  <si>
+    <t>25.4.</t>
+  </si>
+  <si>
+    <t>Tomas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -106,6 +117,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -434,22 +453,22 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -460,7 +479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -471,62 +490,68 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>

</xml_diff>